<commit_message>
ADD MIGRACION DE REPROCESOS INICIO
</commit_message>
<xml_diff>
--- a/mapeo REPROCESOS.xlsx
+++ b/mapeo REPROCESOS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>TABLA</t>
   </si>
@@ -42,6 +42,264 @@
   </si>
   <si>
     <t>Mapeo de datos origen y destino - REPROCESOS</t>
+  </si>
+  <si>
+    <t>NroFormularioRepro</t>
+  </si>
+  <si>
+    <t>IdTipoReproceso</t>
+  </si>
+  <si>
+    <t>IdTipoBeneficio</t>
+  </si>
+  <si>
+    <t>NFormTipoRepro</t>
+  </si>
+  <si>
+    <t>NumeroResolucion</t>
+  </si>
+  <si>
+    <t>FechaResolucion</t>
+  </si>
+  <si>
+    <t>FechaInicioRepro</t>
+  </si>
+  <si>
+    <t>NUP</t>
+  </si>
+  <si>
+    <t>IdTramite</t>
+  </si>
+  <si>
+    <t>IdGrupoBeneficio</t>
+  </si>
+  <si>
+    <t>NoFormularioCalculo</t>
+  </si>
+  <si>
+    <t>IdTipoFormularioCalculo</t>
+  </si>
+  <si>
+    <t>EstadoFormCalcCC</t>
+  </si>
+  <si>
+    <t>VerSalarioCotizable</t>
+  </si>
+  <si>
+    <t>FechaCalculo</t>
+  </si>
+  <si>
+    <t>MontoCC</t>
+  </si>
+  <si>
+    <t>MontoCCNuevo</t>
+  </si>
+  <si>
+    <t>SIP_impresion</t>
+  </si>
+  <si>
+    <t>SIP_impresionNuevo</t>
+  </si>
+  <si>
+    <t>NroCertificado</t>
+  </si>
+  <si>
+    <t>IdTipoTramite</t>
+  </si>
+  <si>
+    <t>IdTipoCC</t>
+  </si>
+  <si>
+    <t>RegistroAPS</t>
+  </si>
+  <si>
+    <t>CursoPago</t>
+  </si>
+  <si>
+    <t>CertificadoAnulado</t>
+  </si>
+  <si>
+    <t>RegistroAPS_Baja</t>
+  </si>
+  <si>
+    <t>NroCertificadoNuevo</t>
+  </si>
+  <si>
+    <t>NumeroEnvioCertificadoNuevo</t>
+  </si>
+  <si>
+    <t>RegistroAPS_Alta</t>
+  </si>
+  <si>
+    <t>FechaNacimiento</t>
+  </si>
+  <si>
+    <t>FechaNacimientoNueva</t>
+  </si>
+  <si>
+    <t>Matricula</t>
+  </si>
+  <si>
+    <t>MatriculaNueva</t>
+  </si>
+  <si>
+    <t>TipoDocumento</t>
+  </si>
+  <si>
+    <t>NumeroDocumento</t>
+  </si>
+  <si>
+    <t>FechaCalculoRepro</t>
+  </si>
+  <si>
+    <t>FechaSolicitud</t>
+  </si>
+  <si>
+    <t>PagoCC</t>
+  </si>
+  <si>
+    <t>SalarioActualizadoRefI</t>
+  </si>
+  <si>
+    <t>MontoActualizadoCCI</t>
+  </si>
+  <si>
+    <t>MontoActualizadoPUI</t>
+  </si>
+  <si>
+    <t>SalarioActualizadoRefII</t>
+  </si>
+  <si>
+    <t>MontoActualizadoCCII</t>
+  </si>
+  <si>
+    <t>MontoActualizadoPUII</t>
+  </si>
+  <si>
+    <t>IdEstadoReproceso</t>
+  </si>
+  <si>
+    <t>FechaCambioEstado</t>
+  </si>
+  <si>
+    <t>RegistroActivo</t>
+  </si>
+  <si>
+    <t>IdUsuario</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>bigint</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde al identificador de la persona, fk a la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Persona.Persona</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde al numero de tramite de CC, fk a la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tramite.TramitePersona</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde al identificador del grupo de beneficio al cual pertenece en CC, va asociado a un numero de tramite, fk a la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tramite.TramitePersona</t>
+    </r>
+  </si>
+  <si>
+    <t>ReprocesoCC</t>
+  </si>
+  <si>
+    <t>Dato propio de la tabla, campo NRO_FORM</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde al clasificador 101: Tipos de Reproceso, fk a la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Clasificador.DetalleClasificador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde a un tipo de beneficio, fk a la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Clasificador.BeneficioOtorgado</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Concatena el Numero de Formulario y el Tipo de Reprocesos </t>
+  </si>
+  <si>
+    <t>Dato propio de la tabla, Numero de Resolucion Administrativa campo NUM_RA</t>
+  </si>
+  <si>
+    <t>Dato propio de la tabla, campo NUM_RA</t>
+  </si>
+  <si>
+    <t>Dato propio de la tabla, campo FECHA</t>
   </si>
 </sst>
 </file>
@@ -76,7 +334,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,8 +347,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -146,25 +416,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,28 +739,28 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -492,365 +783,580 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+    <row r="10" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="E42" s="8"/>
     </row>
     <row r="43" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="5"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
+      <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
+      <c r="E48" s="9"/>
     </row>
     <row r="49" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="5"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="5"/>
+      <c r="A51" s="6"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
+      <c r="A52" s="6"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="5"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
analisis worflow y conclusion dato a dato
</commit_message>
<xml_diff>
--- a/mapeo REPROCESOS.xlsx
+++ b/mapeo REPROCESOS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="92">
   <si>
     <t>TABLA</t>
   </si>
@@ -497,9 +497,6 @@
     </r>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Dato propio de la tabla, campo </t>
     </r>
@@ -545,10 +542,16 @@
     </r>
   </si>
   <si>
-    <t>NO SE CONOCE EL ORIGEN</t>
-  </si>
-  <si>
-    <t>DE DONDE OBTENERLO</t>
+    <t>VERIFICAR SI EXISTE EN LA NUEVA ESTRUCTURA</t>
+  </si>
+  <si>
+    <t>SE COMPLETARA POSTERIORMENTE</t>
+  </si>
+  <si>
+    <t>VERIFICAR CORRESPONDENCIA CON CertificadoCC</t>
+  </si>
+  <si>
+    <t>CONSULTAR EL ORIGEN DE ESTA CAMPO</t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -599,12 +602,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -691,6 +688,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -703,9 +701,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,14 +999,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1033,7 +1029,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1050,7 +1046,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1065,7 +1061,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1080,7 +1076,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1090,10 +1086,15 @@
       <c r="D6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1101,14 +1102,14 @@
         <v>55</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1116,14 +1117,14 @@
         <v>56</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1138,7 +1139,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1153,7 +1154,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1168,7 +1169,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1183,7 +1184,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1198,7 +1199,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1213,7 +1214,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1223,10 +1224,12 @@
       <c r="D15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1236,10 +1239,12 @@
       <c r="D16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1249,10 +1254,12 @@
       <c r="D17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1262,15 +1269,15 @@
       <c r="D18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>90</v>
+      <c r="E18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1280,15 +1287,13 @@
       <c r="D19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="E19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1298,15 +1303,15 @@
       <c r="D20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>90</v>
+      <c r="E20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1316,15 +1321,13 @@
       <c r="D21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="E21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1332,12 +1335,17 @@
         <v>54</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1347,12 +1355,12 @@
       <c r="D23" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1362,10 +1370,12 @@
       <c r="D24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1375,10 +1385,12 @@
       <c r="D25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
@@ -1388,10 +1400,12 @@
       <c r="D26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1401,10 +1415,12 @@
       <c r="D27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="2" t="s">
         <v>31</v>
       </c>
@@ -1414,10 +1430,12 @@
       <c r="D28" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="2" t="s">
         <v>32</v>
       </c>
@@ -1427,10 +1445,12 @@
       <c r="D29" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>33</v>
       </c>
@@ -1440,10 +1460,12 @@
       <c r="D30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1453,10 +1475,12 @@
       <c r="D31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1466,10 +1490,12 @@
       <c r="D32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="8"/>
+      <c r="E32" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1479,10 +1505,12 @@
       <c r="D33" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="8"/>
+      <c r="E33" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="2" t="s">
         <v>37</v>
       </c>
@@ -1492,10 +1520,12 @@
       <c r="D34" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="2" t="s">
         <v>38</v>
       </c>
@@ -1505,10 +1535,12 @@
       <c r="D35" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="2" t="s">
         <v>39</v>
       </c>
@@ -1518,10 +1550,12 @@
       <c r="D36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="2" t="s">
         <v>40</v>
       </c>
@@ -1531,10 +1565,12 @@
       <c r="D37" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="2" t="s">
         <v>41</v>
       </c>
@@ -1549,7 +1585,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="2" t="s">
         <v>42</v>
       </c>
@@ -1564,7 +1600,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="2" t="s">
         <v>43</v>
       </c>
@@ -1579,7 +1615,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="2" t="s">
         <v>44</v>
       </c>
@@ -1594,7 +1630,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="2" t="s">
         <v>45</v>
       </c>
@@ -1609,7 +1645,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
+      <c r="A43" s="7"/>
       <c r="B43" s="2" t="s">
         <v>46</v>
       </c>
@@ -1624,7 +1660,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="2" t="s">
         <v>47</v>
       </c>
@@ -1639,7 +1675,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="6"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="2" t="s">
         <v>48</v>
       </c>
@@ -1654,7 +1690,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="6"/>
+      <c r="A46" s="7"/>
       <c r="B46" s="2" t="s">
         <v>49</v>
       </c>
@@ -1669,7 +1705,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="6"/>
+      <c r="A47" s="7"/>
       <c r="B47" s="2" t="s">
         <v>50</v>
       </c>
@@ -1684,7 +1720,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="6"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="2" t="s">
         <v>51</v>
       </c>
@@ -1692,15 +1728,15 @@
         <v>56</v>
       </c>
       <c r="D48" s="2"/>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F48" s="10" t="s">
-        <v>89</v>
+      <c r="F48" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="6"/>
+      <c r="A49" s="7"/>
       <c r="B49" s="2" t="s">
         <v>52</v>
       </c>
@@ -1715,7 +1751,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
+      <c r="A50" s="8"/>
       <c r="B50" s="2" t="s">
         <v>53</v>
       </c>

</xml_diff>